<commit_message>
oriented load cell connector correctly
</commit_message>
<xml_diff>
--- a/Misc_Projects/Shock_Dyno/ShockDyno2022/Shock Dyno PCB/parts.xlsx
+++ b/Misc_Projects/Shock_Dyno/ShockDyno2022/Shock Dyno PCB/parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GTOR\DAQ\Misc_Projects\Shock_Dyno\ShockDyno2022\Shock Dyno PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C014662-0FD3-41F3-9261-DCE89EA434C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8602C8-E1D0-4094-A6C8-7F85C745E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{39938B10-CD05-4F10-AF73-4316A3DF181E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="132">
   <si>
     <t>Part</t>
   </si>
@@ -448,10 +448,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,14 +482,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
@@ -922,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AF51E6-938E-4D8A-B944-D4099AA8BD5E}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="209" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1470,7 +1481,7 @@
       <c r="N8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1561,8 +1572,8 @@
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>53</v>
+      <c r="B10" s="1">
+        <v>1985195</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -3237,9 +3248,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O8" r:id="rId1" xr:uid="{FACDF33E-80C5-452E-858F-C771F0FCF942}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>